<commit_message>
commited stuff, so integ tests are all passing now, somehow, that was some genius modifications
</commit_message>
<xml_diff>
--- a/integ_tests/partitioning/excel_sheet_for_partition_test_data/traclus_line_partitioning_integration_test_fixture_math.xlsx
+++ b/integ_tests/partitioning/excel_sheet_for_partition_test_data/traclus_line_partitioning_integration_test_fixture_math.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>theta</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>total perp_cost and angle_cost</t>
+  </si>
+  <si>
+    <t>const factor</t>
   </si>
 </sst>
 </file>
@@ -99,7 +102,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8099518810148729E-2"/>
+          <c:x val="5.8099518810148743E-2"/>
           <c:y val="7.4548702245552642E-2"/>
           <c:w val="0.67149759405074361"/>
           <c:h val="0.8326195683872849"/>
@@ -150,22 +153,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-4.7146366481993205</c:v>
+                  <c:v>-7.7512013912860027</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.71023663028961925</c:v>
+                  <c:v>0.25759864453339887</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.91418642625253055</c:v>
+                  <c:v>3.5064447576176985</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9584345865302311</c:v>
+                  <c:v>5.5949410781731004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.736066921261755</c:v>
+                  <c:v>7.1502057476361482</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3614686367055975</c:v>
+                  <c:v>8.4010091785238323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -208,26 +211,100 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>no_par_cost_10</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$9:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.3221478410645684</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3254467148300728</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3327220031906153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3440140701251448</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3593863792411711</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3789269429217872</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>par_cost_10</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$9:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-2.7512013912860027</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2575986445333998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5064447576177002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.5949410781731</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.150205747636148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.401009178523832</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100829440"/>
-        <c:axId val="111150208"/>
+        <c:axId val="120034048"/>
+        <c:axId val="120035584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100829440"/>
+        <c:axId val="120034048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111150208"/>
+        <c:crossAx val="120035584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111150208"/>
+        <c:axId val="120035584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,7 +312,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100829440"/>
+        <c:crossAx val="120034048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -248,7 +325,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -258,16 +335,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -577,7 +654,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -629,20 +706,20 @@
         <v>2.3221478410645684</v>
       </c>
       <c r="K3">
-        <f>2 * (LOG(2 * E3 * SIN(RADIANS(H3)), 2))</f>
-        <v>-7.0365647430866822</v>
+        <f>2 * (2 * LOG(E3 * SIN(RADIANS(H3)), 2))</f>
+        <v>-18.073129486173364</v>
       </c>
       <c r="O3">
         <f>K3</f>
-        <v>-7.0365647430866822</v>
+        <v>-18.073129486173364</v>
       </c>
       <c r="Q3">
         <f>LOG(D3, 2)</f>
         <v>2.3219280948873622</v>
       </c>
       <c r="S3">
-        <f>O3+Q3</f>
-        <v>-4.7146366481993205</v>
+        <f>O3+Q3 + $M$6</f>
+        <v>-7.7512013912860027</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -662,20 +739,20 @@
         <v>2.3254467148300728</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K8" si="2">2 * (LOG(2 * E4 * SIN(RADIANS(H4)), 2))</f>
-        <v>-3.0321647251769814</v>
+        <f t="shared" ref="K4:K20" si="2">2 * (2 * LOG(E4 * SIN(RADIANS(H4)), 2))</f>
+        <v>-10.064329450353963</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O20" si="3">K4</f>
-        <v>-3.0321647251769814</v>
+        <v>-10.064329450353963</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q20" si="4">LOG(D4, 2)</f>
         <v>2.3219280948873622</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S20" si="5">O4+Q4</f>
-        <v>-0.71023663028961925</v>
+        <f t="shared" ref="S4:S20" si="5">O4+Q4 + $M$6</f>
+        <v>0.25759864453339887</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -696,11 +773,14 @@
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>-1.4077416686348316</v>
+        <v>-6.8154833372696633</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
       </c>
       <c r="O5">
         <f t="shared" si="3"/>
-        <v>-1.4077416686348316</v>
+        <v>-6.8154833372696633</v>
       </c>
       <c r="Q5">
         <f t="shared" si="4"/>
@@ -708,7 +788,7 @@
       </c>
       <c r="S5">
         <f t="shared" si="5"/>
-        <v>0.91418642625253055</v>
+        <v>3.5064447576176985</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -729,11 +809,14 @@
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>-0.36349350835713112</v>
+        <v>-4.7269870167142622</v>
+      </c>
+      <c r="M6">
+        <v>8</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>-0.36349350835713112</v>
+        <v>-4.7269870167142622</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
@@ -741,7 +824,7 @@
       </c>
       <c r="S6">
         <f t="shared" si="5"/>
-        <v>1.9584345865302311</v>
+        <v>5.5949410781731004</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -762,11 +845,11 @@
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>0.41413882637439287</v>
+        <v>-3.1717223472512144</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>0.41413882637439287</v>
+        <v>-3.1717223472512144</v>
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
@@ -774,7 +857,7 @@
       </c>
       <c r="S7">
         <f t="shared" si="5"/>
-        <v>2.736066921261755</v>
+        <v>7.1502057476361482</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -795,11 +878,11 @@
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>1.0395405418182353</v>
+        <v>-1.9209189163635296</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>1.0395405418182353</v>
+        <v>-1.9209189163635296</v>
       </c>
       <c r="Q8">
         <f t="shared" si="4"/>
@@ -807,7 +890,7 @@
       </c>
       <c r="S8">
         <f t="shared" si="5"/>
-        <v>3.3614686367055975</v>
+        <v>8.4010091785238323</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -815,31 +898,31 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E4:E20" si="7">D9 / (2 * COS(RADIANS(H9)))</f>
-        <v>5</v>
+        <f t="shared" ref="E9:E20" si="7">D9 / (2 * COS(RADIANS(H9)))</f>
+        <v>5.0007616402195385</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I4:I20" si="8">LOG(2 * E9, 2)</f>
+        <f t="shared" ref="I9:I20" si="8">LOG(2 * E9, 2)</f>
+        <v>3.3221478410645684</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>-14.073129486173364</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>-14.073129486173364</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
         <v>3.3219280948873626</v>
       </c>
-      <c r="K9" t="e">
-        <f t="shared" ref="K4:K20" si="9">2 * (2 * LOG(E9 * SIN(RADIANS(H9)), 2))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O9" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="4"/>
-        <v>3.3219280948873626</v>
-      </c>
-      <c r="S9" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
+      <c r="S9">
+        <f t="shared" si="5"/>
+        <v>-2.7512013912860027</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -848,23 +931,23 @@
       </c>
       <c r="E10">
         <f t="shared" si="7"/>
-        <v>5.019099187716737</v>
+        <v>5.0122094904058612</v>
       </c>
       <c r="H10">
-        <f>H9 + 5</f>
-        <v>5</v>
+        <f>H9+3</f>
+        <v>4</v>
       </c>
       <c r="I10">
         <f t="shared" si="8"/>
-        <v>3.3274284569986161</v>
+        <v>3.3254467148300728</v>
       </c>
       <c r="K10">
-        <f t="shared" si="9"/>
-        <v>-4.771328020775365</v>
+        <f t="shared" si="2"/>
+        <v>-6.0643294503539629</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>-4.771328020775365</v>
+        <v>-6.0643294503539629</v>
       </c>
       <c r="Q10">
         <f t="shared" si="4"/>
@@ -872,7 +955,7 @@
       </c>
       <c r="S10">
         <f t="shared" si="5"/>
-        <v>-1.4493999258880024</v>
+        <v>5.2575986445333998</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -881,23 +964,23 @@
       </c>
       <c r="E11">
         <f t="shared" si="7"/>
-        <v>5.0771330594287249</v>
+        <v>5.0375491272942421</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H14" si="10">H10 + 5</f>
-        <v>10</v>
+        <f t="shared" ref="H11:H14" si="9">H10+3</f>
+        <v>7</v>
       </c>
       <c r="I11">
         <f t="shared" si="8"/>
-        <v>3.3440140701251448</v>
+        <v>3.3327220031906153</v>
       </c>
       <c r="K11">
-        <f t="shared" si="9"/>
-        <v>-0.72698701671426225</v>
+        <f t="shared" si="2"/>
+        <v>-2.8154833372696633</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>-0.72698701671426225</v>
+        <v>-2.8154833372696633</v>
       </c>
       <c r="Q11">
         <f t="shared" si="4"/>
@@ -905,7 +988,7 @@
       </c>
       <c r="S11">
         <f t="shared" si="5"/>
-        <v>2.5949410781731004</v>
+        <v>8.5064447576177002</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -914,23 +997,23 @@
       </c>
       <c r="E12">
         <f t="shared" si="7"/>
-        <v>5.1763809020504148</v>
+        <v>5.0771330594287249</v>
       </c>
       <c r="H12">
-        <f t="shared" si="10"/>
-        <v>15</v>
+        <f t="shared" si="9"/>
+        <v>10</v>
       </c>
       <c r="I12">
         <f t="shared" si="8"/>
-        <v>3.3719437814108666</v>
+        <v>3.3440140701251448</v>
       </c>
       <c r="K12">
-        <f t="shared" si="9"/>
-        <v>1.687837871737482</v>
+        <f t="shared" si="2"/>
+        <v>-0.72698701671426225</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>1.687837871737482</v>
+        <v>-0.72698701671426225</v>
       </c>
       <c r="Q12">
         <f t="shared" si="4"/>
@@ -938,7 +1021,7 @@
       </c>
       <c r="S12">
         <f t="shared" si="5"/>
-        <v>5.0097659666248449</v>
+        <v>10.5949410781731</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -947,23 +1030,23 @@
       </c>
       <c r="E13">
         <f t="shared" si="7"/>
-        <v>5.3208888623795607</v>
+        <v>5.1315205389669583</v>
       </c>
       <c r="H13">
-        <f t="shared" si="10"/>
-        <v>20</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="I13">
         <f t="shared" si="8"/>
-        <v>3.4116672702060158</v>
+        <v>3.3593863792411711</v>
       </c>
       <c r="K13">
-        <f t="shared" si="9"/>
-        <v>3.4552818826580922</v>
+        <f t="shared" si="2"/>
+        <v>0.82827765274878573</v>
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
-        <v>3.4552818826580922</v>
+        <v>0.82827765274878573</v>
       </c>
       <c r="Q13">
         <f t="shared" si="4"/>
@@ -971,7 +1054,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="5"/>
-        <v>6.7772099775454553</v>
+        <v>12.150205747636148</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -980,23 +1063,23 @@
       </c>
       <c r="E14">
         <f t="shared" si="7"/>
-        <v>5.5168895948124588</v>
+        <v>5.20149717930801</v>
       </c>
       <c r="H14">
-        <f t="shared" si="10"/>
-        <v>25</v>
+        <f t="shared" si="9"/>
+        <v>16</v>
       </c>
       <c r="I14">
         <f t="shared" si="8"/>
-        <v>3.4638551092347685</v>
+        <v>3.3789269429217872</v>
       </c>
       <c r="K14">
-        <f t="shared" si="9"/>
-        <v>4.8851284928181551</v>
+        <f t="shared" si="2"/>
+        <v>2.0790810836364706</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>4.8851284928181551</v>
+        <v>2.0790810836364706</v>
       </c>
       <c r="Q14">
         <f t="shared" si="4"/>
@@ -1004,7 +1087,7 @@
       </c>
       <c r="S14">
         <f t="shared" si="5"/>
-        <v>8.2070565877055177</v>
+        <v>13.401009178523832</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1013,30 +1096,30 @@
       </c>
       <c r="E15">
         <f t="shared" si="7"/>
+        <v>1.0001523280439077</v>
+      </c>
+      <c r="H15">
         <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
       </c>
       <c r="I15">
         <f t="shared" si="8"/>
+        <v>1.0002197461772062</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>-23.360841865722815</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>-23.360841865722815</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K15" t="e">
-        <f t="shared" si="9"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O15" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="S15" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
+      <c r="S15">
+        <f t="shared" si="5"/>
+        <v>-14.360841865722815</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1045,23 +1128,23 @@
       </c>
       <c r="E16">
         <f t="shared" si="7"/>
-        <v>1.0038198375433474</v>
+        <v>1.0024418980811722</v>
       </c>
       <c r="H16">
-        <f>H15+5</f>
-        <v>5</v>
+        <f>H15+3</f>
+        <v>4</v>
       </c>
       <c r="I16">
         <f t="shared" si="8"/>
-        <v>1.0055003621112535</v>
+        <v>1.0035186199427106</v>
       </c>
       <c r="K16">
-        <f t="shared" si="9"/>
-        <v>-14.059040400324816</v>
+        <f t="shared" si="2"/>
+        <v>-15.352041829903413</v>
       </c>
       <c r="O16">
         <f t="shared" si="3"/>
-        <v>-14.059040400324816</v>
+        <v>-15.352041829903413</v>
       </c>
       <c r="Q16">
         <f t="shared" si="4"/>
@@ -1069,7 +1152,7 @@
       </c>
       <c r="S16">
         <f t="shared" si="5"/>
-        <v>-13.059040400324816</v>
+        <v>-6.3520418299034134</v>
       </c>
     </row>
     <row r="17" spans="4:19">
@@ -1078,23 +1161,23 @@
       </c>
       <c r="E17">
         <f t="shared" si="7"/>
-        <v>1.0154266118857451</v>
+        <v>1.0075098254588484</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:H20" si="11">H16+5</f>
-        <v>10</v>
+        <f t="shared" ref="H17:H20" si="10">H16+3</f>
+        <v>7</v>
       </c>
       <c r="I17">
         <f t="shared" si="8"/>
-        <v>1.0220859752377829</v>
+        <v>1.0107939083032529</v>
       </c>
       <c r="K17">
-        <f t="shared" si="9"/>
-        <v>-10.014699396263712</v>
+        <f t="shared" si="2"/>
+        <v>-12.103195716819112</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>-10.014699396263712</v>
+        <v>-12.103195716819112</v>
       </c>
       <c r="Q17">
         <f t="shared" si="4"/>
@@ -1102,7 +1185,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="5"/>
-        <v>-9.0146993962637119</v>
+        <v>-3.103195716819112</v>
       </c>
     </row>
     <row r="18" spans="4:19">
@@ -1111,23 +1194,23 @@
       </c>
       <c r="E18">
         <f t="shared" si="7"/>
-        <v>1.035276180410083</v>
+        <v>1.0154266118857451</v>
       </c>
       <c r="H18">
-        <f t="shared" si="11"/>
-        <v>15</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="I18">
         <f t="shared" si="8"/>
-        <v>1.050015686523504</v>
+        <v>1.0220859752377829</v>
       </c>
       <c r="K18">
-        <f t="shared" si="9"/>
-        <v>-7.5998745078119692</v>
+        <f t="shared" si="2"/>
+        <v>-10.014699396263712</v>
       </c>
       <c r="O18">
         <f t="shared" si="3"/>
-        <v>-7.5998745078119692</v>
+        <v>-10.014699396263712</v>
       </c>
       <c r="Q18">
         <f t="shared" si="4"/>
@@ -1135,7 +1218,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="5"/>
-        <v>-6.5998745078119692</v>
+        <v>-1.0146993962637119</v>
       </c>
     </row>
     <row r="19" spans="4:19">
@@ -1144,23 +1227,23 @@
       </c>
       <c r="E19">
         <f t="shared" si="7"/>
-        <v>1.0641777724759121</v>
+        <v>1.0263041077933917</v>
       </c>
       <c r="H19">
-        <f t="shared" si="11"/>
-        <v>20</v>
+        <f t="shared" si="10"/>
+        <v>13</v>
       </c>
       <c r="I19">
         <f t="shared" si="8"/>
-        <v>1.0897391753186536</v>
+        <v>1.0374582843538083</v>
       </c>
       <c r="K19">
-        <f t="shared" si="9"/>
-        <v>-5.8324304968913578</v>
+        <f t="shared" si="2"/>
+        <v>-8.459434726800664</v>
       </c>
       <c r="O19">
         <f t="shared" si="3"/>
-        <v>-5.8324304968913578</v>
+        <v>-8.459434726800664</v>
       </c>
       <c r="Q19">
         <f t="shared" si="4"/>
@@ -1168,7 +1251,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="5"/>
-        <v>-4.8324304968913578</v>
+        <v>0.540565273199336</v>
       </c>
     </row>
     <row r="20" spans="4:19">
@@ -1177,23 +1260,23 @@
       </c>
       <c r="E20">
         <f t="shared" si="7"/>
-        <v>1.1033779189624917</v>
+        <v>1.040299435861602</v>
       </c>
       <c r="H20">
-        <f t="shared" si="11"/>
-        <v>25</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="I20">
         <f t="shared" si="8"/>
-        <v>1.1419270143474063</v>
+        <v>1.0569988480344248</v>
       </c>
       <c r="K20">
-        <f t="shared" si="9"/>
-        <v>-4.4025838867312945</v>
+        <f t="shared" si="2"/>
+        <v>-7.2086312959129799</v>
       </c>
       <c r="O20">
         <f t="shared" si="3"/>
-        <v>-4.4025838867312945</v>
+        <v>-7.2086312959129799</v>
       </c>
       <c r="Q20">
         <f t="shared" si="4"/>
@@ -1201,7 +1284,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="5"/>
-        <v>-3.4025838867312945</v>
+        <v>1.7913687040870201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lifted the restriction that line segments must be greater than 1 in length. realized that the super negative offset from perp and angular distance (log of them), offset the fact that sum of logs less than log of sum for values less than 2
</commit_message>
<xml_diff>
--- a/integ_tests/partitioning/excel_sheet_for_partition_test_data/traclus_line_partitioning_integration_test_fixture_math.xlsx
+++ b/integ_tests/partitioning/excel_sheet_for_partition_test_data/traclus_line_partitioning_integration_test_fixture_math.xlsx
@@ -153,22 +153,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-7.7512013912860027</c:v>
+                  <c:v>-4.7146366481993205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25759864453339887</c:v>
+                  <c:v>-0.71023663028961925</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5064447576176985</c:v>
+                  <c:v>0.91418642625253055</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5949410781731004</c:v>
+                  <c:v>1.9584345865302311</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1502057476361482</c:v>
+                  <c:v>2.736066921261755</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4010091785238323</c:v>
+                  <c:v>3.3614686367055975</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -264,22 +264,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-2.7512013912860027</c:v>
+                  <c:v>-1.7146366481993196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2575986445333998</c:v>
+                  <c:v>2.2897633697103812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.5064447576177002</c:v>
+                  <c:v>3.914186426252531</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.5949410781731</c:v>
+                  <c:v>4.9584345865302319</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.150205747636148</c:v>
+                  <c:v>5.7360669212617559</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.401009178523832</c:v>
+                  <c:v>6.3614686367055988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,16 +335,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -654,7 +654,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F6" sqref="F6:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,12 +706,12 @@
         <v>2.3221478410645684</v>
       </c>
       <c r="K3">
-        <f>2 * (2 * LOG(E3 * SIN(RADIANS(H3)), 2))</f>
-        <v>-18.073129486173364</v>
+        <f>2 * (LOG(2 * E3 * SIN(RADIANS(H3)), 2))</f>
+        <v>-7.0365647430866822</v>
       </c>
       <c r="O3">
         <f>K3</f>
-        <v>-18.073129486173364</v>
+        <v>-7.0365647430866822</v>
       </c>
       <c r="Q3">
         <f>LOG(D3, 2)</f>
@@ -719,7 +719,7 @@
       </c>
       <c r="S3">
         <f>O3+Q3 + $M$6</f>
-        <v>-7.7512013912860027</v>
+        <v>-4.7146366481993205</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -739,12 +739,12 @@
         <v>2.3254467148300728</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K20" si="2">2 * (2 * LOG(E4 * SIN(RADIANS(H4)), 2))</f>
-        <v>-10.064329450353963</v>
+        <f t="shared" ref="K4:K20" si="2">2 * (LOG(2 * E4 * SIN(RADIANS(H4)), 2))</f>
+        <v>-3.0321647251769814</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O20" si="3">K4</f>
-        <v>-10.064329450353963</v>
+        <v>-3.0321647251769814</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q20" si="4">LOG(D4, 2)</f>
@@ -752,7 +752,7 @@
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S20" si="5">O4+Q4 + $M$6</f>
-        <v>0.25759864453339887</v>
+        <v>-0.71023663028961925</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -773,14 +773,14 @@
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>-6.8154833372696633</v>
+        <v>-1.4077416686348316</v>
       </c>
       <c r="M5" t="s">
         <v>9</v>
       </c>
       <c r="O5">
         <f t="shared" si="3"/>
-        <v>-6.8154833372696633</v>
+        <v>-1.4077416686348316</v>
       </c>
       <c r="Q5">
         <f t="shared" si="4"/>
@@ -788,7 +788,7 @@
       </c>
       <c r="S5">
         <f t="shared" si="5"/>
-        <v>3.5064447576176985</v>
+        <v>0.91418642625253055</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -809,14 +809,14 @@
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>-4.7269870167142622</v>
+        <v>-0.36349350835713112</v>
       </c>
       <c r="M6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>-4.7269870167142622</v>
+        <v>-0.36349350835713112</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="S6">
         <f t="shared" si="5"/>
-        <v>5.5949410781731004</v>
+        <v>1.9584345865302311</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -845,11 +845,11 @@
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>-3.1717223472512144</v>
+        <v>0.41413882637439287</v>
       </c>
       <c r="O7">
         <f t="shared" si="3"/>
-        <v>-3.1717223472512144</v>
+        <v>0.41413882637439287</v>
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
@@ -857,7 +857,7 @@
       </c>
       <c r="S7">
         <f t="shared" si="5"/>
-        <v>7.1502057476361482</v>
+        <v>2.736066921261755</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -878,11 +878,11 @@
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>-1.9209189163635296</v>
+        <v>1.0395405418182353</v>
       </c>
       <c r="O8">
         <f t="shared" si="3"/>
-        <v>-1.9209189163635296</v>
+        <v>1.0395405418182353</v>
       </c>
       <c r="Q8">
         <f t="shared" si="4"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="S8">
         <f t="shared" si="5"/>
-        <v>8.4010091785238323</v>
+        <v>3.3614686367055975</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -910,11 +910,11 @@
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>-14.073129486173364</v>
+        <v>-5.0365647430866822</v>
       </c>
       <c r="O9">
         <f t="shared" si="3"/>
-        <v>-14.073129486173364</v>
+        <v>-5.0365647430866822</v>
       </c>
       <c r="Q9">
         <f t="shared" si="4"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="S9">
         <f t="shared" si="5"/>
-        <v>-2.7512013912860027</v>
+        <v>-1.7146366481993196</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -943,11 +943,11 @@
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>-6.0643294503539629</v>
+        <v>-1.0321647251769814</v>
       </c>
       <c r="O10">
         <f t="shared" si="3"/>
-        <v>-6.0643294503539629</v>
+        <v>-1.0321647251769814</v>
       </c>
       <c r="Q10">
         <f t="shared" si="4"/>
@@ -955,7 +955,7 @@
       </c>
       <c r="S10">
         <f t="shared" si="5"/>
-        <v>5.2575986445333998</v>
+        <v>2.2897633697103812</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -976,11 +976,11 @@
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>-2.8154833372696633</v>
+        <v>0.59225833136516848</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
-        <v>-2.8154833372696633</v>
+        <v>0.59225833136516848</v>
       </c>
       <c r="Q11">
         <f t="shared" si="4"/>
@@ -988,7 +988,7 @@
       </c>
       <c r="S11">
         <f t="shared" si="5"/>
-        <v>8.5064447576177002</v>
+        <v>3.914186426252531</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1009,11 +1009,11 @@
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>-0.72698701671426225</v>
+        <v>1.6365064916428691</v>
       </c>
       <c r="O12">
         <f t="shared" si="3"/>
-        <v>-0.72698701671426225</v>
+        <v>1.6365064916428691</v>
       </c>
       <c r="Q12">
         <f t="shared" si="4"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="S12">
         <f t="shared" si="5"/>
-        <v>10.5949410781731</v>
+        <v>4.9584345865302319</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1042,11 +1042,11 @@
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>0.82827765274878573</v>
+        <v>2.4141388263743928</v>
       </c>
       <c r="O13">
         <f t="shared" si="3"/>
-        <v>0.82827765274878573</v>
+        <v>2.4141388263743928</v>
       </c>
       <c r="Q13">
         <f t="shared" si="4"/>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="5"/>
-        <v>12.150205747636148</v>
+        <v>5.7360669212617559</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>2.0790810836364706</v>
+        <v>3.0395405418182357</v>
       </c>
       <c r="O14">
         <f t="shared" si="3"/>
-        <v>2.0790810836364706</v>
+        <v>3.0395405418182357</v>
       </c>
       <c r="Q14">
         <f t="shared" si="4"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="S14">
         <f t="shared" si="5"/>
-        <v>13.401009178523832</v>
+        <v>6.3614686367055988</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1107,11 +1107,11 @@
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>-23.360841865722815</v>
+        <v>-9.6804209328614075</v>
       </c>
       <c r="O15">
         <f t="shared" si="3"/>
-        <v>-23.360841865722815</v>
+        <v>-9.6804209328614075</v>
       </c>
       <c r="Q15">
         <f t="shared" si="4"/>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="S15">
         <f t="shared" si="5"/>
-        <v>-14.360841865722815</v>
+        <v>-8.6804209328614075</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>-15.352041829903413</v>
+        <v>-5.6760209149517058</v>
       </c>
       <c r="O16">
         <f t="shared" si="3"/>
-        <v>-15.352041829903413</v>
+        <v>-5.6760209149517058</v>
       </c>
       <c r="Q16">
         <f t="shared" si="4"/>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="S16">
         <f t="shared" si="5"/>
-        <v>-6.3520418299034134</v>
+        <v>-4.6760209149517058</v>
       </c>
     </row>
     <row r="17" spans="4:19">
@@ -1173,11 +1173,11 @@
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
-        <v>-12.103195716819112</v>
+        <v>-4.051597858409556</v>
       </c>
       <c r="O17">
         <f t="shared" si="3"/>
-        <v>-12.103195716819112</v>
+        <v>-4.051597858409556</v>
       </c>
       <c r="Q17">
         <f t="shared" si="4"/>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="5"/>
-        <v>-3.103195716819112</v>
+        <v>-3.051597858409556</v>
       </c>
     </row>
     <row r="18" spans="4:19">
@@ -1206,11 +1206,11 @@
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>-10.014699396263712</v>
+        <v>-3.0073496981318555</v>
       </c>
       <c r="O18">
         <f t="shared" si="3"/>
-        <v>-10.014699396263712</v>
+        <v>-3.0073496981318555</v>
       </c>
       <c r="Q18">
         <f t="shared" si="4"/>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="5"/>
-        <v>-1.0146993962637119</v>
+        <v>-2.0073496981318555</v>
       </c>
     </row>
     <row r="19" spans="4:19">
@@ -1239,11 +1239,11 @@
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
-        <v>-8.459434726800664</v>
+        <v>-2.229717363400332</v>
       </c>
       <c r="O19">
         <f t="shared" si="3"/>
-        <v>-8.459434726800664</v>
+        <v>-2.229717363400332</v>
       </c>
       <c r="Q19">
         <f t="shared" si="4"/>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="5"/>
-        <v>0.540565273199336</v>
+        <v>-1.229717363400332</v>
       </c>
     </row>
     <row r="20" spans="4:19">
@@ -1272,11 +1272,11 @@
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>-7.2086312959129799</v>
+        <v>-1.6043156479564897</v>
       </c>
       <c r="O20">
         <f t="shared" si="3"/>
-        <v>-7.2086312959129799</v>
+        <v>-1.6043156479564897</v>
       </c>
       <c r="Q20">
         <f t="shared" si="4"/>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="5"/>
-        <v>1.7913687040870201</v>
+        <v>-0.60431564795648973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>